<commit_message>
edit index.html and fix style.css
</commit_message>
<xml_diff>
--- a/Visualisasi.xlsx
+++ b/Visualisasi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Syifa\Downloads\Merge\san-kai.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ACAF38-DD5D-4B2F-A5EA-35000202C0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1F8AD3-5621-4EF3-956D-3CFB5BD05F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23445" yWindow="-1830" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="5" xr2:uid="{708E8231-D815-4126-B8B4-9E6AB9027B75}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7785" firstSheet="3" activeTab="4" xr2:uid="{708E8231-D815-4126-B8B4-9E6AB9027B75}"/>
   </bookViews>
   <sheets>
     <sheet name="JUMLAH PESERTA TIAP TAHUN" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Tahun</t>
   </si>
@@ -94,19 +94,25 @@
     <t>Tender Batal</t>
   </si>
   <si>
-    <t>Jenis Pengadaan</t>
-  </si>
-  <si>
     <t>Jumlah Pengadaan</t>
   </si>
   <si>
-    <t>Pekerjaan Konstruksi</t>
-  </si>
-  <si>
-    <t>Pengadaan Barang</t>
-  </si>
-  <si>
     <t>RATA RATA HARGA PENAWARAN</t>
+  </si>
+  <si>
+    <t>2017 (Pekerjaan Konstruksi)</t>
+  </si>
+  <si>
+    <t>2018 (Pekerjaan Konstruksi</t>
+  </si>
+  <si>
+    <t>2019 (Pengadaan Barang)</t>
+  </si>
+  <si>
+    <t>2020 (Pengadaan Barang)</t>
+  </si>
+  <si>
+    <t>2021 (Pekerjaan Konstruksi)</t>
   </si>
 </sst>
 </file>
@@ -153,10 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,81 +800,64 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C785DE06-FDC9-40F0-A108-BF2F508D4AAC}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2017</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
+      <c r="B2" s="3">
         <v>512</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2018</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3">
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2019</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3">
         <v>337</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2020</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2021</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3">
         <v>228</v>
       </c>
     </row>
@@ -880,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8BEA-856A-4A20-979F-9683636E143C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -894,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>